<commit_message>
Changed ttest+ANOVA input file
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/result_ANOVA.xlsx
+++ b/tests/testthat/testdata/result_ANOVA.xlsx
@@ -575,10 +575,10 @@
         <v>23</v>
       </c>
       <c r="C2" t="n">
+        <v>40866162</v>
+      </c>
+      <c r="D2" t="n">
         <v>34910128</v>
-      </c>
-      <c r="D2" t="e">
-        <v>#N/A</v>
       </c>
       <c r="E2" t="n">
         <v>33763808</v>
@@ -602,31 +602,31 @@
         <v>39887340</v>
       </c>
       <c r="L2" t="n">
-        <v>0.726130274131189</v>
+        <v>0.189475379927987</v>
       </c>
       <c r="M2" t="n">
-        <v>0.806811415701321</v>
-      </c>
-      <c r="N2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O2" t="e">
-        <v>#N/A</v>
+        <v>0.521057294801966</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.20287773784929</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.296429832844544</v>
       </c>
       <c r="P2" t="n">
-        <v>0.726130274131189</v>
+        <v>0.949792502045769</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.830879512485705</v>
+        <v>0.883543583151899</v>
       </c>
       <c r="R2" t="n">
-        <v>1.20354393744569</v>
+        <v>1.13180608072854</v>
       </c>
       <c r="S2" t="n">
-        <v>0.846626098446834</v>
+        <v>0.900288243206019</v>
       </c>
       <c r="T2" t="n">
-        <v>1.18115895769636</v>
+        <v>1.11075536923474</v>
       </c>
       <c r="U2" t="n">
         <v>1.01895170806898</v>
@@ -643,10 +643,10 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
+        <v>200506080</v>
+      </c>
+      <c r="D3" t="n">
         <v>228724928</v>
-      </c>
-      <c r="D3" t="e">
-        <v>#N/A</v>
       </c>
       <c r="E3" t="n">
         <v>230557560</v>
@@ -670,31 +670,31 @@
         <v>287809476</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0244164028947448</v>
+        <v>0.0201658877478581</v>
       </c>
       <c r="M3" t="n">
-        <v>0.225191224151068</v>
-      </c>
-      <c r="N3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O3" t="e">
-        <v>#N/A</v>
+        <v>0.22182476522644</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.832139145277655</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.0228590793007388</v>
       </c>
       <c r="P3" t="n">
-        <v>0.0244164028947448</v>
+        <v>0.0458911123431448</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.013228129569</v>
+        <v>0.970377859861055</v>
       </c>
       <c r="R3" t="n">
-        <v>0.986944569359093</v>
+        <v>1.03052639735946</v>
       </c>
       <c r="S3" t="n">
-        <v>0.854422884967179</v>
+        <v>0.818288622606085</v>
       </c>
       <c r="T3" t="n">
-        <v>1.1703806365608</v>
+        <v>1.22206269569678</v>
       </c>
       <c r="U3" t="n">
         <v>0.843268026254487</v>
@@ -711,10 +711,10 @@
         <v>27</v>
       </c>
       <c r="C4" t="n">
+        <v>26963010</v>
+      </c>
+      <c r="D4" t="n">
         <v>25142570</v>
-      </c>
-      <c r="D4" t="e">
-        <v>#N/A</v>
       </c>
       <c r="E4" t="n">
         <v>24140170</v>
@@ -738,31 +738,31 @@
         <v>26086670</v>
       </c>
       <c r="L4" t="n">
-        <v>0.491319731890592</v>
+        <v>0.542297691644648</v>
       </c>
       <c r="M4" t="n">
-        <v>0.701885331272274</v>
-      </c>
-      <c r="N4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O4" t="e">
-        <v>#N/A</v>
+        <v>0.718415415341795</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.560789044415445</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.987090744506795</v>
       </c>
       <c r="P4" t="n">
-        <v>0.491319731890592</v>
+        <v>0.646685897327063</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.600767574436792</v>
+        <v>0.619635113478052</v>
       </c>
       <c r="R4" t="n">
-        <v>1.66453723960965</v>
+        <v>1.61385302131594</v>
       </c>
       <c r="S4" t="n">
-        <v>0.924931794451845</v>
+        <v>0.953979944659823</v>
       </c>
       <c r="T4" t="n">
-        <v>1.08116080125956</v>
+        <v>1.04824006583974</v>
       </c>
       <c r="U4" t="n">
         <v>1.53958341596407</v>
@@ -793,8 +793,8 @@
       <c r="G5" t="e">
         <v>#N/A</v>
       </c>
-      <c r="H5" t="e">
-        <v>#N/A</v>
+      <c r="H5" t="n">
+        <v>51412512</v>
       </c>
       <c r="I5" t="e">
         <v>#N/A</v>
@@ -915,10 +915,10 @@
         <v>33</v>
       </c>
       <c r="C7" t="n">
+        <v>21140340</v>
+      </c>
+      <c r="D7" t="n">
         <v>23729240</v>
-      </c>
-      <c r="D7" t="e">
-        <v>#N/A</v>
       </c>
       <c r="E7" t="n">
         <v>22417890</v>
@@ -942,31 +942,31 @@
         <v>22170380</v>
       </c>
       <c r="L7" t="n">
-        <v>0.570666844274274</v>
+        <v>0.810948095071544</v>
       </c>
       <c r="M7" t="n">
-        <v>0.713333555342842</v>
-      </c>
-      <c r="N7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O7" t="e">
-        <v>#N/A</v>
+        <v>0.892042904578699</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.983600942601009</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.890278678396742</v>
       </c>
       <c r="P7" t="n">
-        <v>0.570666844274274</v>
+        <v>0.806011276621718</v>
       </c>
       <c r="Q7" t="n">
-        <v>1.03785828203943</v>
+        <v>1.00887253468027</v>
       </c>
       <c r="R7" t="n">
-        <v>0.963522686387359</v>
+        <v>0.991205494871482</v>
       </c>
       <c r="S7" t="n">
-        <v>1.00425848036413</v>
+        <v>0.976211122551528</v>
       </c>
       <c r="T7" t="n">
-        <v>0.995759577392282</v>
+        <v>1.02436857857785</v>
       </c>
       <c r="U7" t="n">
         <v>0.967625828827732</v>
@@ -983,10 +983,10 @@
         <v>35</v>
       </c>
       <c r="C8" t="n">
+        <v>29319660</v>
+      </c>
+      <c r="D8" t="n">
         <v>36068288</v>
-      </c>
-      <c r="D8" t="e">
-        <v>#N/A</v>
       </c>
       <c r="E8" t="n">
         <v>38500928</v>
@@ -1009,14 +1009,14 @@
       <c r="K8" t="n">
         <v>36233440</v>
       </c>
-      <c r="L8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N8" t="e">
-        <v>#N/A</v>
+      <c r="L8" t="n">
+        <v>0.185574458134091</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.521057294801966</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.185574458134091</v>
       </c>
       <c r="O8" t="e">
         <v>#N/A</v>
@@ -1024,23 +1024,23 @@
       <c r="P8" t="e">
         <v>#N/A</v>
       </c>
-      <c r="Q8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="R8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="S8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="T8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="U8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="V8" t="e">
-        <v>#N/A</v>
+      <c r="Q8" t="n">
+        <v>0.879108622783973</v>
+      </c>
+      <c r="R8" t="n">
+        <v>1.13751585877202</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.943844831357479</v>
+      </c>
+      <c r="T8" t="n">
+        <v>1.05949618706049</v>
+      </c>
+      <c r="U8" t="n">
+        <v>1.07363846388914</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.931412233851618</v>
       </c>
     </row>
     <row r="9">
@@ -1051,10 +1051,10 @@
         <v>37</v>
       </c>
       <c r="C9" t="n">
+        <v>34100360</v>
+      </c>
+      <c r="D9" t="n">
         <v>37990528</v>
-      </c>
-      <c r="D9" t="e">
-        <v>#N/A</v>
       </c>
       <c r="E9" t="n">
         <v>32654220</v>
@@ -1078,31 +1078,31 @@
         <v>34394968</v>
       </c>
       <c r="L9" t="n">
-        <v>0.925005576772831</v>
+        <v>0.981726057366263</v>
       </c>
       <c r="M9" t="n">
-        <v>0.925005576772831</v>
-      </c>
-      <c r="N9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O9" t="e">
-        <v>#N/A</v>
+        <v>0.981726057366263</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.994654180225996</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.9798818297913</v>
       </c>
       <c r="P9" t="n">
-        <v>0.925005576772831</v>
+        <v>0.995176795604732</v>
       </c>
       <c r="Q9" t="n">
-        <v>1.00542692903801</v>
+        <v>0.993832334789599</v>
       </c>
       <c r="R9" t="n">
-        <v>0.99460236355197</v>
+        <v>1.00620594137914</v>
       </c>
       <c r="S9" t="n">
-        <v>1.00245376544802</v>
+        <v>0.99089345775437</v>
       </c>
       <c r="T9" t="n">
-        <v>0.997552240778985</v>
+        <v>1.0091902334952</v>
       </c>
       <c r="U9" t="n">
         <v>0.99704288446617</v>
@@ -1119,10 +1119,10 @@
         <v>39</v>
       </c>
       <c r="C10" t="n">
+        <v>2663829782</v>
+      </c>
+      <c r="D10" t="n">
         <v>2590670618</v>
-      </c>
-      <c r="D10" t="e">
-        <v>#N/A</v>
       </c>
       <c r="E10" t="n">
         <v>2707158182</v>
@@ -1146,31 +1146,31 @@
         <v>2587524814</v>
       </c>
       <c r="L10" t="n">
-        <v>0.347116046822432</v>
+        <v>0.127775914975779</v>
       </c>
       <c r="M10" t="n">
-        <v>0.701885331272274</v>
-      </c>
-      <c r="N10" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O10" t="e">
-        <v>#N/A</v>
+        <v>0.521057294801966</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.111398617213416</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.478315521734763</v>
       </c>
       <c r="P10" t="n">
-        <v>0.347116046822432</v>
+        <v>0.496419426256647</v>
       </c>
       <c r="Q10" t="n">
-        <v>1.06493039599863</v>
+        <v>1.06692918257824</v>
       </c>
       <c r="R10" t="n">
-        <v>0.939028507175115</v>
+        <v>0.937269329894508</v>
       </c>
       <c r="S10" t="n">
-        <v>1.03071624831247</v>
+        <v>1.03265081775687</v>
       </c>
       <c r="T10" t="n">
-        <v>0.970199122830596</v>
+        <v>0.968381550476288</v>
       </c>
       <c r="U10" t="n">
         <v>0.967871939973993</v>
@@ -1186,11 +1186,11 @@
       <c r="B11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D11" t="n">
         <v>1495972</v>
-      </c>
-      <c r="D11" t="e">
-        <v>#N/A</v>
       </c>
       <c r="E11" t="e">
         <v>#N/A</v>
@@ -1217,7 +1217,7 @@
         <v>0.474443964389275</v>
       </c>
       <c r="M11" t="n">
-        <v>0.701885331272274</v>
+        <v>0.718415415341795</v>
       </c>
       <c r="N11" t="e">
         <v>#N/A</v>
@@ -1255,10 +1255,10 @@
         <v>43</v>
       </c>
       <c r="C12" t="n">
+        <v>36614408</v>
+      </c>
+      <c r="D12" t="n">
         <v>52227550</v>
-      </c>
-      <c r="D12" t="e">
-        <v>#N/A</v>
       </c>
       <c r="E12" t="n">
         <v>52181250</v>
@@ -1282,31 +1282,31 @@
         <v>53973140</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0450382448302136</v>
+        <v>0.553929488510475</v>
       </c>
       <c r="M12" t="n">
-        <v>0.225191224151068</v>
-      </c>
-      <c r="N12" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O12" t="e">
-        <v>#N/A</v>
+        <v>0.718415415341795</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.90895745541081</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.532037995358854</v>
       </c>
       <c r="P12" t="n">
-        <v>0.0450382448302136</v>
+        <v>0.766443509189862</v>
       </c>
       <c r="Q12" t="n">
-        <v>1.07973150623046</v>
+        <v>0.972250109105049</v>
       </c>
       <c r="R12" t="n">
-        <v>0.926156173298292</v>
+        <v>1.02854192623387</v>
       </c>
       <c r="S12" t="n">
-        <v>1.00643820679858</v>
+        <v>0.906252758876663</v>
       </c>
       <c r="T12" t="n">
-        <v>0.993602978548425</v>
+        <v>1.10344491666932</v>
       </c>
       <c r="U12" t="n">
         <v>0.932118958269764</v>
@@ -1391,10 +1391,10 @@
         <v>47</v>
       </c>
       <c r="C14" t="n">
+        <v>49490460</v>
+      </c>
+      <c r="D14" t="n">
         <v>49514448</v>
-      </c>
-      <c r="D14" t="e">
-        <v>#N/A</v>
       </c>
       <c r="E14" t="n">
         <v>50004128</v>
@@ -1418,31 +1418,31 @@
         <v>43506848</v>
       </c>
       <c r="L14" t="n">
-        <v>0.419218589807043</v>
+        <v>0.509443342858738</v>
       </c>
       <c r="M14" t="n">
-        <v>0.701885331272274</v>
-      </c>
-      <c r="N14" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O14" t="e">
-        <v>#N/A</v>
+        <v>0.718415415341795</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.997063924126177</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.588597745217175</v>
       </c>
       <c r="P14" t="n">
-        <v>0.419218589807043</v>
+        <v>0.548478562918217</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.997725836950765</v>
+        <v>0.99592907597021</v>
       </c>
       <c r="R14" t="n">
-        <v>1.00227934665517</v>
+        <v>1.00408756419309</v>
       </c>
       <c r="S14" t="n">
-        <v>1.04742388975689</v>
+        <v>1.04553762971879</v>
       </c>
       <c r="T14" t="n">
-        <v>0.954723307134137</v>
+        <v>0.956445728566421</v>
       </c>
       <c r="U14" t="n">
         <v>1.04981133189656</v>
@@ -1458,11 +1458,11 @@
       <c r="B15" t="s">
         <v>49</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D15" t="n">
         <v>15940000</v>
-      </c>
-      <c r="D15" t="e">
-        <v>#N/A</v>
       </c>
       <c r="E15" t="e">
         <v>#N/A</v>
@@ -1527,10 +1527,10 @@
         <v>51</v>
       </c>
       <c r="C16" t="n">
+        <v>64759632</v>
+      </c>
+      <c r="D16" t="n">
         <v>53367728</v>
-      </c>
-      <c r="D16" t="e">
-        <v>#N/A</v>
       </c>
       <c r="E16" t="n">
         <v>60332520</v>
@@ -1554,31 +1554,31 @@
         <v>62191500</v>
       </c>
       <c r="L16" t="n">
-        <v>0.227983278314776</v>
+        <v>0.587794430734196</v>
       </c>
       <c r="M16" t="n">
-        <v>0.701885331272274</v>
-      </c>
-      <c r="N16" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O16" t="e">
-        <v>#N/A</v>
+        <v>0.718415415341795</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.873873701444645</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.560643554844047</v>
       </c>
       <c r="P16" t="n">
-        <v>0.227983278314776</v>
+        <v>0.83689440554514</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.935173364478294</v>
+        <v>0.978543315074051</v>
       </c>
       <c r="R16" t="n">
-        <v>1.06932044686481</v>
+        <v>1.02192716928869</v>
       </c>
       <c r="S16" t="n">
-        <v>0.909495289288623</v>
+        <v>0.95167438384135</v>
       </c>
       <c r="T16" t="n">
-        <v>1.09951091751357</v>
+        <v>1.05077957017566</v>
       </c>
       <c r="U16" t="n">
         <v>0.972541909163553</v>

</xml_diff>

<commit_message>
shortened some protein names, because they were throwing a NOTE for being too long
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/result_ANOVA.xlsx
+++ b/tests/testthat/testdata/result_ANOVA.xlsx
@@ -95,7 +95,7 @@
     <t xml:space="preserve">FEAHPNDLYVEGLPENIPFR</t>
   </si>
   <si>
-    <t xml:space="preserve">G3UYD0/G3UYJ6/Q3UHU8/Q9ESZ8</t>
+    <t xml:space="preserve">G3UYD0/G3UYJ6/Q3UHU8</t>
   </si>
   <si>
     <t xml:space="preserve">LPNSVLGR</t>
@@ -137,7 +137,7 @@
     <t xml:space="preserve">QHIEKAK</t>
   </si>
   <si>
-    <t xml:space="preserve">A0A087WPR7/A0A087WSP0/E9Q9X1/Q91ZU6/S4R1P5</t>
+    <t xml:space="preserve">A0A087WPR7/A0A087WSP0/E9Q9X1</t>
   </si>
   <si>
     <t xml:space="preserve">RLDETPDGRK</t>
@@ -161,7 +161,7 @@
     <t xml:space="preserve">VVAGVANALAHK</t>
   </si>
   <si>
-    <t xml:space="preserve">contaminant_HBB_HUMAN/P02042/P68871</t>
+    <t xml:space="preserve">contaminant_HBB_HUMAN/P02042</t>
   </si>
   <si>
     <t xml:space="preserve">YTPLYPFR</t>

</xml_diff>